<commit_message>
Made The First UI Changes.
</commit_message>
<xml_diff>
--- a/Speak2Sheet/Assets/Excel Tests/ΒΑΘΜΟΛΟΓΙΟ Εξόρυξη Γνώσης και Συστήματα Λήψης Αποφάσεων (Ε705) 2020-2021 ΣΕΠΤΕΜΒΡΙΟΣ.xlsx
+++ b/Speak2Sheet/Assets/Excel Tests/ΒΑΘΜΟΛΟΓΙΟ Εξόρυξη Γνώσης και Συστήματα Λήψης Αποφάσεων (Ε705) 2020-2021 ΣΕΠΤΕΜΒΡΙΟΣ.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
     <t xml:space="preserve">Αριθμός Μητρώου</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
   </si>
 </sst>
 </file>
@@ -701,6 +704,9 @@
       <c r="G8" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="H8" s="0" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="0" t="s">

</xml_diff>

<commit_message>
Fixed the ExcelLoader build issue, added the dll needed for excel encoding and exposed certain variables to work the options functionalities
</commit_message>
<xml_diff>
--- a/Speak2Sheet/Assets/Excel Tests/ΒΑΘΜΟΛΟΓΙΟ Εξόρυξη Γνώσης και Συστήματα Λήψης Αποφάσεων (Ε705) 2020-2021 ΣΕΠΤΕΜΒΡΙΟΣ.xlsx
+++ b/Speak2Sheet/Assets/Excel Tests/ΒΑΘΜΟΛΟΓΙΟ Εξόρυξη Γνώσης και Συστήματα Λήψης Αποφάσεων (Ε705) 2020-2021 ΣΕΠΤΕΜΒΡΙΟΣ.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
   <si>
     <t xml:space="preserve">Αριθμός Μητρώου</t>
   </si>
@@ -601,6 +601,9 @@
       <c r="G3" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="H3" s="0" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="0" t="s">

</xml_diff>